<commit_message>
Added analysis for close types
</commit_message>
<xml_diff>
--- a/females_and_males_on_males_means.xlsx
+++ b/females_and_males_on_males_means.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shlomin\PycharmProjects\lda_test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB625383-2A3A-4F46-B02D-EFA938A9323E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69AF442E-EA30-4B31-821A-D15BA5227332}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="19120" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="males_on_females_and_males_mean" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Determined</t>
   </si>
@@ -72,11 +73,20 @@
   <si>
     <t>Males</t>
   </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>effect</t>
+  </si>
+  <si>
+    <t>marginal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1718,16 +1728,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>568678</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>54328</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2051,11 +2061,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2207,6 +2217,107 @@
         <v>5.4846539651285699E-2</v>
       </c>
     </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>12.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>51.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>111.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>15.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>29.14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>88.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>41.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>32.07</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>11.13</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>7.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>